<commit_message>
Aggiornamento della repository con nuovi risultati
</commit_message>
<xml_diff>
--- a/Cluster1.xlsx
+++ b/Cluster1.xlsx
@@ -692,1801 +692,1801 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13.79617687500226</v>
+        <v>13.51687330175527</v>
       </c>
       <c r="B2" t="n">
-        <v>12.85957088839511</v>
+        <v>12.19095462054962</v>
       </c>
       <c r="C2" t="n">
-        <v>11.95834482280747</v>
+        <v>11.74976300791305</v>
       </c>
       <c r="D2" t="n">
-        <v>11.51216819944841</v>
+        <v>11.46487165925586</v>
       </c>
       <c r="E2" t="n">
-        <v>12.57792169331558</v>
+        <v>12.7757022477421</v>
       </c>
       <c r="F2" t="n">
-        <v>12.26749354733429</v>
+        <v>12.40583985936862</v>
       </c>
       <c r="G2" t="n">
-        <v>12.28197489411816</v>
+        <v>12.49311153386715</v>
       </c>
       <c r="H2" t="n">
-        <v>12.68120764341524</v>
+        <v>12.78808540094465</v>
       </c>
       <c r="I2" t="n">
-        <v>12.98224262384786</v>
+        <v>13.17316104489463</v>
       </c>
       <c r="J2" t="n">
-        <v>12.49062746083958</v>
+        <v>12.64509427871351</v>
       </c>
       <c r="K2" t="n">
-        <v>12.11615236006647</v>
+        <v>12.30436071019098</v>
       </c>
       <c r="L2" t="n">
-        <v>12.15225995547123</v>
+        <v>12.58879531797622</v>
       </c>
       <c r="M2" t="n">
-        <v>12.07555824606112</v>
+        <v>12.5049657923295</v>
       </c>
       <c r="N2" t="n">
-        <v>13.1711180572252</v>
+        <v>13.31584244580723</v>
       </c>
       <c r="O2" t="n">
-        <v>11.08632085335447</v>
+        <v>11.72308166838923</v>
       </c>
       <c r="P2" t="n">
-        <v>11.73987099113007</v>
+        <v>12.14208421222713</v>
       </c>
       <c r="Q2" t="n">
-        <v>14.87681217351836</v>
+        <v>14.31044098188312</v>
       </c>
       <c r="R2" t="n">
-        <v>12.13341288757075</v>
+        <v>12.54652275684913</v>
       </c>
       <c r="S2" t="n">
-        <v>12.51286211589015</v>
+        <v>12.94027861830178</v>
       </c>
       <c r="T2" t="n">
-        <v>12.60782628368668</v>
+        <v>12.98704272350902</v>
       </c>
       <c r="U2" t="n">
-        <v>11.32099265246394</v>
+        <v>11.88247883612414</v>
       </c>
       <c r="V2" t="n">
-        <v>11.45324885112228</v>
+        <v>12.01241085685622</v>
       </c>
       <c r="W2" t="n">
-        <v>11.36363479836586</v>
+        <v>11.91061071948102</v>
       </c>
       <c r="X2" t="n">
-        <v>12.42037064219697</v>
+        <v>12.75103078079366</v>
       </c>
       <c r="Y2" t="n">
-        <v>12.50157266769961</v>
+        <v>13.03650486909778</v>
       </c>
       <c r="Z2" t="n">
-        <v>12.31698650563082</v>
+        <v>12.70665700112515</v>
       </c>
       <c r="AA2" t="n">
-        <v>12.27350064720638</v>
+        <v>12.59199676536088</v>
       </c>
       <c r="AB2" t="n">
-        <v>12.22063751119514</v>
+        <v>12.60927993845084</v>
       </c>
       <c r="AC2" t="n">
-        <v>10.93555467070452</v>
+        <v>11.55151420483867</v>
       </c>
       <c r="AD2" t="n">
-        <v>12.46527408883413</v>
+        <v>13.03347798531779</v>
       </c>
       <c r="AE2" t="n">
-        <v>12.31721242752702</v>
+        <v>12.63842123483509</v>
       </c>
       <c r="AF2" t="n">
-        <v>13.01493358730408</v>
+        <v>13.28044457069372</v>
       </c>
       <c r="AG2" t="n">
-        <v>12.97931104208126</v>
+        <v>13.18904689083481</v>
       </c>
       <c r="AH2" t="n">
-        <v>13.34846084308846</v>
+        <v>13.3685450674119</v>
       </c>
       <c r="AI2" t="n">
-        <v>11.90498861210136</v>
+        <v>12.31833822214391</v>
       </c>
       <c r="AJ2" t="n">
-        <v>12.14752267275961</v>
+        <v>12.48322630814388</v>
       </c>
       <c r="AK2" t="n">
-        <v>12.41735208152221</v>
+        <v>12.69602230453833</v>
       </c>
       <c r="AL2" t="n">
-        <v>12.42935670827868</v>
+        <v>12.78928368841794</v>
       </c>
       <c r="AM2" t="n">
-        <v>11.74820784319028</v>
+        <v>12.15202566654509</v>
       </c>
       <c r="AN2" t="n">
-        <v>11.89933497575607</v>
+        <v>12.38115863510251</v>
       </c>
       <c r="AO2" t="n">
-        <v>12.82233706970806</v>
+        <v>13.08329848639493</v>
       </c>
       <c r="AP2" t="n">
-        <v>12.02236139758216</v>
+        <v>12.33368691621725</v>
       </c>
       <c r="AQ2" t="n">
-        <v>12.09905049765438</v>
+        <v>12.48918791799593</v>
       </c>
       <c r="AR2" t="n">
-        <v>12.29774521463114</v>
+        <v>12.53967501102495</v>
       </c>
       <c r="AS2" t="n">
-        <v>15.47464352928004</v>
+        <v>15.19467343591401</v>
       </c>
       <c r="AT2" t="n">
-        <v>13.6262774267884</v>
+        <v>13.61918902124853</v>
       </c>
       <c r="AU2" t="n">
-        <v>11.98696843195969</v>
+        <v>12.32064073236198</v>
       </c>
       <c r="AV2" t="n">
-        <v>11.97925920656523</v>
+        <v>12.35568733908722</v>
       </c>
       <c r="AW2" t="n">
-        <v>13.13395879908605</v>
+        <v>13.18572548906729</v>
       </c>
       <c r="AX2" t="n">
-        <v>11.64481193712663</v>
+        <v>12.14474454815059</v>
       </c>
       <c r="AY2" t="n">
-        <v>12.55622947958484</v>
+        <v>12.87680029520834</v>
       </c>
       <c r="AZ2" t="n">
-        <v>12.40088569319468</v>
+        <v>12.55669413726248</v>
       </c>
       <c r="BA2" t="n">
-        <v>11.91988754184355</v>
+        <v>12.26861313656439</v>
       </c>
       <c r="BB2" t="n">
-        <v>11.89170031411257</v>
+        <v>12.29719110565393</v>
       </c>
       <c r="BC2" t="n">
-        <v>12.67206571802277</v>
+        <v>12.93155415528289</v>
       </c>
       <c r="BD2" t="n">
-        <v>12.73185052877376</v>
+        <v>12.93264598204713</v>
       </c>
       <c r="BE2" t="n">
-        <v>12.55219143750087</v>
+        <v>12.91644342751624</v>
       </c>
       <c r="BF2" t="n">
-        <v>12.41166047640624</v>
+        <v>12.60179534521452</v>
       </c>
       <c r="BG2" t="n">
-        <v>12.20982715814909</v>
+        <v>12.30055274431405</v>
       </c>
       <c r="BH2" t="n">
-        <v>12.33072431160518</v>
+        <v>12.56688721067893</v>
       </c>
       <c r="BI2" t="n">
-        <v>12.43743709243101</v>
+        <v>12.75158329707024</v>
       </c>
       <c r="BJ2" t="n">
-        <v>12.29797775866897</v>
+        <v>12.67660761903855</v>
       </c>
       <c r="BK2" t="n">
-        <v>11.7930539719842</v>
+        <v>12.2881336692527</v>
       </c>
       <c r="BL2" t="n">
-        <v>12.70998615118696</v>
+        <v>12.95425967216522</v>
       </c>
       <c r="BM2" t="n">
-        <v>12.31983909377096</v>
+        <v>12.7304261691951</v>
       </c>
       <c r="BN2" t="n">
-        <v>12.37519853892976</v>
+        <v>12.60825285068806</v>
       </c>
       <c r="BO2" t="n">
-        <v>11.8543912167041</v>
+        <v>12.39234859456783</v>
       </c>
       <c r="BP2" t="n">
-        <v>12.27116323192985</v>
+        <v>12.73531385136706</v>
       </c>
       <c r="BQ2" t="n">
-        <v>12.08893503673206</v>
+        <v>12.3317738968903</v>
       </c>
       <c r="BR2" t="n">
-        <v>12.14027123527906</v>
+        <v>12.41916325356622</v>
       </c>
       <c r="BS2" t="n">
-        <v>12.33132213775789</v>
+        <v>12.55431787665884</v>
       </c>
       <c r="BT2" t="n">
-        <v>12.06826160767704</v>
+        <v>12.4550152126156</v>
       </c>
       <c r="BU2" t="n">
-        <v>12.68105872975418</v>
+        <v>13.06881539758944</v>
       </c>
       <c r="BV2" t="n">
-        <v>13.51438656421065</v>
+        <v>13.49429444811976</v>
       </c>
       <c r="BW2" t="n">
-        <v>12.0221085698493</v>
+        <v>12.31915486742348</v>
       </c>
       <c r="BX2" t="n">
-        <v>12.69106079034721</v>
+        <v>12.87829876311892</v>
       </c>
       <c r="BY2" t="n">
-        <v>12.17517146707684</v>
+        <v>12.44925009487444</v>
       </c>
       <c r="BZ2" t="n">
-        <v>12.3932921332844</v>
+        <v>12.59136932532229</v>
       </c>
       <c r="CA2" t="n">
-        <v>12.66756697205552</v>
+        <v>12.83202629392326</v>
       </c>
       <c r="CB2" t="n">
-        <v>12.69354595614253</v>
+        <v>12.95275273066131</v>
       </c>
       <c r="CC2" t="n">
-        <v>11.84101910802628</v>
+        <v>12.12004305422206</v>
       </c>
       <c r="CD2" t="n">
-        <v>12.58367469248698</v>
+        <v>12.67684167381393</v>
       </c>
       <c r="CE2" t="n">
-        <v>12.30488661846038</v>
+        <v>12.65641651884537</v>
       </c>
       <c r="CF2" t="n">
-        <v>13.28683740609511</v>
+        <v>13.429130519529</v>
       </c>
       <c r="CG2" t="n">
-        <v>12.18795345106515</v>
+        <v>12.57979415632162</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>14.01224791457427</v>
+        <v>13.81694089406254</v>
       </c>
       <c r="B3" t="n">
-        <v>12.23960217809074</v>
+        <v>11.60722952874038</v>
       </c>
       <c r="C3" t="n">
-        <v>12.19801359781171</v>
+        <v>12.06390868406346</v>
       </c>
       <c r="D3" t="n">
-        <v>11.41464842765754</v>
+        <v>11.42973549652387</v>
       </c>
       <c r="E3" t="n">
-        <v>12.4327287257033</v>
+        <v>12.72241160028196</v>
       </c>
       <c r="F3" t="n">
-        <v>12.2515639220887</v>
+        <v>12.45969551075154</v>
       </c>
       <c r="G3" t="n">
-        <v>12.6937593600487</v>
+        <v>12.91153937631469</v>
       </c>
       <c r="H3" t="n">
-        <v>12.43500305960533</v>
+        <v>12.59737545608035</v>
       </c>
       <c r="I3" t="n">
-        <v>13.11439287452015</v>
+        <v>13.37497594191279</v>
       </c>
       <c r="J3" t="n">
-        <v>12.17283376746581</v>
+        <v>12.42647117435678</v>
       </c>
       <c r="K3" t="n">
-        <v>11.96185380275039</v>
+        <v>12.23841830018226</v>
       </c>
       <c r="L3" t="n">
-        <v>12.11326181610081</v>
+        <v>12.63678607081343</v>
       </c>
       <c r="M3" t="n">
-        <v>12.12037879321122</v>
+        <v>12.62539507813082</v>
       </c>
       <c r="N3" t="n">
-        <v>12.77886173527259</v>
+        <v>12.98264814408903</v>
       </c>
       <c r="O3" t="n">
-        <v>11.40541462300235</v>
+        <v>12.05651146156264</v>
       </c>
       <c r="P3" t="n">
-        <v>12.01686025458067</v>
+        <v>12.45710401288114</v>
       </c>
       <c r="Q3" t="n">
-        <v>14.3977905568805</v>
+        <v>13.89994868836085</v>
       </c>
       <c r="R3" t="n">
-        <v>12.0794175287693</v>
+        <v>12.55791990475699</v>
       </c>
       <c r="S3" t="n">
-        <v>12.72790464965469</v>
+        <v>13.20899906634973</v>
       </c>
       <c r="T3" t="n">
-        <v>12.71153999116253</v>
+        <v>13.13874377539645</v>
       </c>
       <c r="U3" t="n">
-        <v>11.45112176101595</v>
+        <v>12.08821610830609</v>
       </c>
       <c r="V3" t="n">
-        <v>11.5731533892381</v>
+        <v>12.18269143762852</v>
       </c>
       <c r="W3" t="n">
-        <v>11.47191284874833</v>
+        <v>12.03980874939262</v>
       </c>
       <c r="X3" t="n">
-        <v>12.3269489860638</v>
+        <v>12.74104312154918</v>
       </c>
       <c r="Y3" t="n">
-        <v>13.24600080328156</v>
+        <v>13.75663476057529</v>
       </c>
       <c r="Z3" t="n">
-        <v>12.18136820877756</v>
+        <v>12.64247763428929</v>
       </c>
       <c r="AA3" t="n">
-        <v>12.1160078286474</v>
+        <v>12.52978270877965</v>
       </c>
       <c r="AB3" t="n">
-        <v>12.20176035744194</v>
+        <v>12.65300898969743</v>
       </c>
       <c r="AC3" t="n">
-        <v>11.09724588470472</v>
+        <v>11.78436586232565</v>
       </c>
       <c r="AD3" t="n">
-        <v>13.19161141001854</v>
+        <v>13.76327493386911</v>
       </c>
       <c r="AE3" t="n">
-        <v>12.06496886549722</v>
+        <v>12.44989884624068</v>
       </c>
       <c r="AF3" t="n">
-        <v>12.6386317764644</v>
+        <v>12.97593445479186</v>
       </c>
       <c r="AG3" t="n">
-        <v>12.58992762819284</v>
+        <v>12.87751759029387</v>
       </c>
       <c r="AH3" t="n">
-        <v>13.0513405994943</v>
+        <v>13.08096767252475</v>
       </c>
       <c r="AI3" t="n">
-        <v>11.89697381763432</v>
+        <v>12.35238254039799</v>
       </c>
       <c r="AJ3" t="n">
-        <v>11.98973935152963</v>
+        <v>12.38112427825758</v>
       </c>
       <c r="AK3" t="n">
-        <v>12.11241771117561</v>
+        <v>12.46125413778354</v>
       </c>
       <c r="AL3" t="n">
-        <v>12.21877731336072</v>
+        <v>12.64281598688572</v>
       </c>
       <c r="AM3" t="n">
-        <v>11.70318746376902</v>
+        <v>12.19444145381672</v>
       </c>
       <c r="AN3" t="n">
-        <v>12.12404928482514</v>
+        <v>12.64938316708611</v>
       </c>
       <c r="AO3" t="n">
-        <v>12.45282532100356</v>
+        <v>12.78487348177659</v>
       </c>
       <c r="AP3" t="n">
-        <v>11.87930547914791</v>
+        <v>12.24041231874516</v>
       </c>
       <c r="AQ3" t="n">
-        <v>11.94785757298679</v>
+        <v>12.37322060325652</v>
       </c>
       <c r="AR3" t="n">
-        <v>12.08756958183635</v>
+        <v>12.38620600249516</v>
       </c>
       <c r="AS3" t="n">
-        <v>14.85839858029566</v>
+        <v>14.59108325723639</v>
       </c>
       <c r="AT3" t="n">
-        <v>13.13107665039911</v>
+        <v>13.21052033268416</v>
       </c>
       <c r="AU3" t="n">
-        <v>11.84568721365998</v>
+        <v>12.25935947941745</v>
       </c>
       <c r="AV3" t="n">
-        <v>11.90413302742755</v>
+        <v>12.33936585723686</v>
       </c>
       <c r="AW3" t="n">
-        <v>12.7049243481464</v>
+        <v>12.83199305308644</v>
       </c>
       <c r="AX3" t="n">
-        <v>11.81552754037195</v>
+        <v>12.3862119042721</v>
       </c>
       <c r="AY3" t="n">
-        <v>12.27268240401683</v>
+        <v>12.65029487469434</v>
       </c>
       <c r="AZ3" t="n">
-        <v>12.15550056957795</v>
+        <v>12.39392923984084</v>
       </c>
       <c r="BA3" t="n">
-        <v>11.78622552540211</v>
+        <v>12.20543205518564</v>
       </c>
       <c r="BB3" t="n">
-        <v>11.75384643439025</v>
+        <v>12.20306825133593</v>
       </c>
       <c r="BC3" t="n">
-        <v>12.33821125036358</v>
+        <v>12.66440889977685</v>
       </c>
       <c r="BD3" t="n">
-        <v>12.44451651300168</v>
+        <v>12.67661024217545</v>
       </c>
       <c r="BE3" t="n">
-        <v>12.2720446719632</v>
+        <v>12.68327616328085</v>
       </c>
       <c r="BF3" t="n">
-        <v>12.24716760992553</v>
+        <v>12.47695411359731</v>
       </c>
       <c r="BG3" t="n">
-        <v>12.00445798861173</v>
+        <v>12.16139877238492</v>
       </c>
       <c r="BH3" t="n">
-        <v>12.07914019511388</v>
+        <v>12.39953577932127</v>
       </c>
       <c r="BI3" t="n">
-        <v>12.17732423841059</v>
+        <v>12.55102523650159</v>
       </c>
       <c r="BJ3" t="n">
-        <v>12.09612837352643</v>
+        <v>12.52785681399096</v>
       </c>
       <c r="BK3" t="n">
-        <v>12.0049838376534</v>
+        <v>12.54497048205531</v>
       </c>
       <c r="BL3" t="n">
-        <v>12.44666883494455</v>
+        <v>12.74675334233487</v>
       </c>
       <c r="BM3" t="n">
-        <v>12.31777031323131</v>
+        <v>12.7948514332789</v>
       </c>
       <c r="BN3" t="n">
-        <v>12.13439037197998</v>
+        <v>12.43077052745647</v>
       </c>
       <c r="BO3" t="n">
-        <v>12.01460056245091</v>
+        <v>12.60694871373314</v>
       </c>
       <c r="BP3" t="n">
-        <v>12.53541207082217</v>
+        <v>13.06683655880963</v>
       </c>
       <c r="BQ3" t="n">
-        <v>11.92687764762054</v>
+        <v>12.24235310731366</v>
       </c>
       <c r="BR3" t="n">
-        <v>11.94181807805825</v>
+        <v>12.29831842269208</v>
       </c>
       <c r="BS3" t="n">
-        <v>12.13400595667491</v>
+        <v>12.42105964087477</v>
       </c>
       <c r="BT3" t="n">
-        <v>12.06267502287457</v>
+        <v>12.53263303042236</v>
       </c>
       <c r="BU3" t="n">
-        <v>13.12674905937327</v>
+        <v>13.53631028331957</v>
       </c>
       <c r="BV3" t="n">
-        <v>13.09271231819135</v>
+        <v>13.12737565044328</v>
       </c>
       <c r="BW3" t="n">
-        <v>11.84431188975476</v>
+        <v>12.20150982568547</v>
       </c>
       <c r="BX3" t="n">
-        <v>12.37171878434087</v>
+        <v>12.61477369813995</v>
       </c>
       <c r="BY3" t="n">
-        <v>11.96898199848929</v>
+        <v>12.31735987667759</v>
       </c>
       <c r="BZ3" t="n">
-        <v>12.13332394830996</v>
+        <v>12.40346104914917</v>
       </c>
       <c r="CA3" t="n">
-        <v>12.35881685426295</v>
+        <v>12.56264443364784</v>
       </c>
       <c r="CB3" t="n">
-        <v>12.3805353752125</v>
+        <v>12.70628506334256</v>
       </c>
       <c r="CC3" t="n">
-        <v>11.71196650883468</v>
+        <v>12.07136467400158</v>
       </c>
       <c r="CD3" t="n">
-        <v>12.25304391657346</v>
+        <v>12.45719601227247</v>
       </c>
       <c r="CE3" t="n">
-        <v>12.22418870431157</v>
+        <v>12.6509210308522</v>
       </c>
       <c r="CF3" t="n">
-        <v>12.85032348341857</v>
+        <v>13.06954929785104</v>
       </c>
       <c r="CG3" t="n">
-        <v>12.04841525930825</v>
+        <v>12.51702169883757</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>15.01270961427067</v>
+        <v>14.76920718344937</v>
       </c>
       <c r="B4" t="n">
-        <v>13.31475983389111</v>
+        <v>12.62949831085777</v>
       </c>
       <c r="C4" t="n">
-        <v>13.2240570031418</v>
+        <v>13.02241732530373</v>
       </c>
       <c r="D4" t="n">
-        <v>12.04840359148121</v>
+        <v>12.0678800179508</v>
       </c>
       <c r="E4" t="n">
-        <v>13.45653814233687</v>
+        <v>13.7915852306047</v>
       </c>
       <c r="F4" t="n">
-        <v>12.72287677440345</v>
+        <v>12.95579356963975</v>
       </c>
       <c r="G4" t="n">
-        <v>13.13317323001766</v>
+        <v>13.34598258277182</v>
       </c>
       <c r="H4" t="n">
-        <v>12.68189532788116</v>
+        <v>12.89702203501761</v>
       </c>
       <c r="I4" t="n">
-        <v>13.97304990252599</v>
+        <v>14.13908672886015</v>
       </c>
       <c r="J4" t="n">
-        <v>12.6993684524193</v>
+        <v>12.90948489297696</v>
       </c>
       <c r="K4" t="n">
-        <v>12.45279694972344</v>
+        <v>12.71520177657302</v>
       </c>
       <c r="L4" t="n">
-        <v>12.41700842946516</v>
+        <v>12.94102180998559</v>
       </c>
       <c r="M4" t="n">
-        <v>12.54916968895758</v>
+        <v>13.04073742112736</v>
       </c>
       <c r="N4" t="n">
-        <v>12.87607584382318</v>
+        <v>13.11839940287751</v>
       </c>
       <c r="O4" t="n">
-        <v>11.22528107949263</v>
+        <v>11.85175138487116</v>
       </c>
       <c r="P4" t="n">
-        <v>11.73044299150464</v>
+        <v>12.16744922619452</v>
       </c>
       <c r="Q4" t="n">
-        <v>14.77030971034974</v>
+        <v>14.25834943558439</v>
       </c>
       <c r="R4" t="n">
-        <v>12.36720238700651</v>
+        <v>12.79367249902133</v>
       </c>
       <c r="S4" t="n">
-        <v>13.28288398192361</v>
+        <v>13.6766881805983</v>
       </c>
       <c r="T4" t="n">
-        <v>12.79459041113584</v>
+        <v>13.19706546568839</v>
       </c>
       <c r="U4" t="n">
-        <v>11.43809704491288</v>
+        <v>12.0227194398108</v>
       </c>
       <c r="V4" t="n">
-        <v>11.60336370583897</v>
+        <v>12.17388669652922</v>
       </c>
       <c r="W4" t="n">
-        <v>11.4802790949039</v>
+        <v>12.04105059566542</v>
       </c>
       <c r="X4" t="n">
-        <v>12.71752920254158</v>
+        <v>13.04803318103447</v>
       </c>
       <c r="Y4" t="n">
-        <v>13.32855394174022</v>
+        <v>13.80222671392255</v>
       </c>
       <c r="Z4" t="n">
-        <v>12.5224301791579</v>
+        <v>12.93249745656875</v>
       </c>
       <c r="AA4" t="n">
-        <v>12.37117888666649</v>
+        <v>12.72582136110173</v>
       </c>
       <c r="AB4" t="n">
-        <v>12.53079644493574</v>
+        <v>12.90123499206701</v>
       </c>
       <c r="AC4" t="n">
-        <v>11.14536689621185</v>
+        <v>11.77609569281531</v>
       </c>
       <c r="AD4" t="n">
-        <v>13.50217121061443</v>
+        <v>13.99382445953496</v>
       </c>
       <c r="AE4" t="n">
-        <v>12.43653255200249</v>
+        <v>12.77191539001391</v>
       </c>
       <c r="AF4" t="n">
-        <v>13.35877653987991</v>
+        <v>13.61598516729602</v>
       </c>
       <c r="AG4" t="n">
-        <v>13.03202183499911</v>
+        <v>13.28438474272725</v>
       </c>
       <c r="AH4" t="n">
-        <v>12.9735629831381</v>
+        <v>13.06669302784284</v>
       </c>
       <c r="AI4" t="n">
-        <v>12.08551091944659</v>
+        <v>12.49703221445465</v>
       </c>
       <c r="AJ4" t="n">
-        <v>12.33380278394741</v>
+        <v>12.66339691787912</v>
       </c>
       <c r="AK4" t="n">
-        <v>12.46774396923672</v>
+        <v>12.77152358000277</v>
       </c>
       <c r="AL4" t="n">
-        <v>12.59792149857427</v>
+        <v>12.9589344240298</v>
       </c>
       <c r="AM4" t="n">
-        <v>11.89833111560449</v>
+        <v>12.31293242870524</v>
       </c>
       <c r="AN4" t="n">
-        <v>12.35352009835429</v>
+        <v>12.80529459883189</v>
       </c>
       <c r="AO4" t="n">
-        <v>12.77724769157262</v>
+        <v>13.07973639464276</v>
       </c>
       <c r="AP4" t="n">
-        <v>11.9387271879007</v>
+        <v>12.28862660920096</v>
       </c>
       <c r="AQ4" t="n">
-        <v>12.09093140997655</v>
+        <v>12.50099090835634</v>
       </c>
       <c r="AR4" t="n">
-        <v>12.29371120730042</v>
+        <v>12.58505972385787</v>
       </c>
       <c r="AS4" t="n">
-        <v>15.32280357875416</v>
+        <v>15.08909166593727</v>
       </c>
       <c r="AT4" t="n">
-        <v>13.48108289396333</v>
+        <v>13.54450751245894</v>
       </c>
       <c r="AU4" t="n">
-        <v>12.01483223292934</v>
+        <v>12.37619228565331</v>
       </c>
       <c r="AV4" t="n">
-        <v>12.16162749101162</v>
+        <v>12.5311683841354</v>
       </c>
       <c r="AW4" t="n">
-        <v>13.0297707697698</v>
+        <v>13.13498707316927</v>
       </c>
       <c r="AX4" t="n">
-        <v>11.95589731296895</v>
+        <v>12.44204855834239</v>
       </c>
       <c r="AY4" t="n">
-        <v>12.65772266769582</v>
+        <v>12.99448851369203</v>
       </c>
       <c r="AZ4" t="n">
-        <v>12.33375383852126</v>
+        <v>12.5451481348617</v>
       </c>
       <c r="BA4" t="n">
-        <v>11.9996920630245</v>
+        <v>12.37300482945756</v>
       </c>
       <c r="BB4" t="n">
-        <v>11.93790652226519</v>
+        <v>12.36268814619032</v>
       </c>
       <c r="BC4" t="n">
-        <v>12.66400018193396</v>
+        <v>12.95831423744099</v>
       </c>
       <c r="BD4" t="n">
-        <v>12.63274053218543</v>
+        <v>12.88313068605915</v>
       </c>
       <c r="BE4" t="n">
-        <v>12.62483891563532</v>
+        <v>13.00049432585798</v>
       </c>
       <c r="BF4" t="n">
-        <v>12.33759230897737</v>
+        <v>12.57359419697916</v>
       </c>
       <c r="BG4" t="n">
-        <v>12.14274649803578</v>
+        <v>12.28228040000191</v>
       </c>
       <c r="BH4" t="n">
-        <v>12.33698411893724</v>
+        <v>12.61421075207191</v>
       </c>
       <c r="BI4" t="n">
-        <v>12.51482260273747</v>
+        <v>12.84040879928075</v>
       </c>
       <c r="BJ4" t="n">
-        <v>12.41753203799511</v>
+        <v>12.81368221667313</v>
       </c>
       <c r="BK4" t="n">
-        <v>12.14514196086884</v>
+        <v>12.59629902953936</v>
       </c>
       <c r="BL4" t="n">
-        <v>12.61598715460167</v>
+        <v>12.91265227015458</v>
       </c>
       <c r="BM4" t="n">
-        <v>12.6609312899199</v>
+        <v>13.05531215649615</v>
       </c>
       <c r="BN4" t="n">
-        <v>12.31685729155271</v>
+        <v>12.59547643282982</v>
       </c>
       <c r="BO4" t="n">
-        <v>12.23995025944457</v>
+        <v>12.76870291112892</v>
       </c>
       <c r="BP4" t="n">
-        <v>12.88998063632038</v>
+        <v>13.3399118492875</v>
       </c>
       <c r="BQ4" t="n">
-        <v>12.25003162353867</v>
+        <v>12.48622327528011</v>
       </c>
       <c r="BR4" t="n">
-        <v>12.17446401580457</v>
+        <v>12.48389767111189</v>
       </c>
       <c r="BS4" t="n">
-        <v>12.26113058090854</v>
+        <v>12.53194920474485</v>
       </c>
       <c r="BT4" t="n">
-        <v>12.33980720703562</v>
+        <v>12.72304777718568</v>
       </c>
       <c r="BU4" t="n">
-        <v>13.48548714332434</v>
+        <v>13.80648895005429</v>
       </c>
       <c r="BV4" t="n">
-        <v>13.37138483795552</v>
+        <v>13.41358890377283</v>
       </c>
       <c r="BW4" t="n">
-        <v>12.02526357315043</v>
+        <v>12.34504681034542</v>
       </c>
       <c r="BX4" t="n">
-        <v>12.6082707302768</v>
+        <v>12.85231301241912</v>
       </c>
       <c r="BY4" t="n">
-        <v>12.20523328638243</v>
+        <v>12.49903710175856</v>
       </c>
       <c r="BZ4" t="n">
-        <v>12.33615884031468</v>
+        <v>12.59333670700548</v>
       </c>
       <c r="CA4" t="n">
-        <v>12.57449679543628</v>
+        <v>12.78712287872326</v>
       </c>
       <c r="CB4" t="n">
-        <v>12.63231082727574</v>
+        <v>12.93419929986603</v>
       </c>
       <c r="CC4" t="n">
-        <v>11.84103670433524</v>
+        <v>12.15886685504758</v>
       </c>
       <c r="CD4" t="n">
-        <v>12.58648926546543</v>
+        <v>12.73388986199256</v>
       </c>
       <c r="CE4" t="n">
-        <v>12.60609314603044</v>
+        <v>12.95436247375601</v>
       </c>
       <c r="CF4" t="n">
-        <v>13.18546996540131</v>
+        <v>13.3829055895514</v>
       </c>
       <c r="CG4" t="n">
-        <v>12.28576095887575</v>
+        <v>12.69704645829215</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>15.20132268971876</v>
+        <v>15.01887035204695</v>
       </c>
       <c r="B5" t="n">
-        <v>12.90823153180783</v>
+        <v>12.2905581536441</v>
       </c>
       <c r="C5" t="n">
-        <v>13.66414586830139</v>
+        <v>13.52696820288493</v>
       </c>
       <c r="D5" t="n">
-        <v>12.5192080665154</v>
+        <v>12.66534328572017</v>
       </c>
       <c r="E5" t="n">
-        <v>13.74368686665816</v>
+        <v>14.28294069040877</v>
       </c>
       <c r="F5" t="n">
-        <v>13.58231902612192</v>
+        <v>13.97450764362327</v>
       </c>
       <c r="G5" t="n">
-        <v>14.26246564663459</v>
+        <v>14.55151750765767</v>
       </c>
       <c r="H5" t="n">
-        <v>13.6015624246306</v>
+        <v>14.00380571982267</v>
       </c>
       <c r="I5" t="n">
-        <v>14.33648134724207</v>
+        <v>14.66686755813546</v>
       </c>
       <c r="J5" t="n">
-        <v>13.10356479815177</v>
+        <v>13.54654238448719</v>
       </c>
       <c r="K5" t="n">
-        <v>13.00272800343107</v>
+        <v>13.53158896821085</v>
       </c>
       <c r="L5" t="n">
-        <v>13.22676315721196</v>
+        <v>13.88525106511431</v>
       </c>
       <c r="M5" t="n">
-        <v>13.23752001974329</v>
+        <v>13.86427778824116</v>
       </c>
       <c r="N5" t="n">
-        <v>13.78226156379477</v>
+        <v>14.21131717795703</v>
       </c>
       <c r="O5" t="n">
-        <v>12.51319378526044</v>
+        <v>13.19639637560616</v>
       </c>
       <c r="P5" t="n">
-        <v>13.24315596839484</v>
+        <v>13.70884837205779</v>
       </c>
       <c r="Q5" t="n">
-        <v>15.15807097155884</v>
+        <v>15.01136903352296</v>
       </c>
       <c r="R5" t="n">
-        <v>13.05317803021307</v>
+        <v>13.62983947659668</v>
       </c>
       <c r="S5" t="n">
-        <v>13.91634677810539</v>
+        <v>14.45104614017591</v>
       </c>
       <c r="T5" t="n">
-        <v>13.88636824235539</v>
+        <v>14.38937506335315</v>
       </c>
       <c r="U5" t="n">
-        <v>12.39462784969255</v>
+        <v>13.08808614855027</v>
       </c>
       <c r="V5" t="n">
-        <v>12.61562034322884</v>
+        <v>13.27752789658447</v>
       </c>
       <c r="W5" t="n">
-        <v>12.61903343153828</v>
+        <v>13.26872729401562</v>
       </c>
       <c r="X5" t="n">
-        <v>13.28121560028947</v>
+        <v>13.79620472918566</v>
       </c>
       <c r="Y5" t="n">
-        <v>14.36746781408112</v>
+        <v>14.8667378841327</v>
       </c>
       <c r="Z5" t="n">
-        <v>13.17943861843934</v>
+        <v>13.7586791493241</v>
       </c>
       <c r="AA5" t="n">
-        <v>13.11905443878092</v>
+        <v>13.63482134817417</v>
       </c>
       <c r="AB5" t="n">
-        <v>13.19199982218654</v>
+        <v>13.72738972994572</v>
       </c>
       <c r="AC5" t="n">
-        <v>12.15052167154839</v>
+        <v>12.87016537787859</v>
       </c>
       <c r="AD5" t="n">
-        <v>14.24505450853802</v>
+        <v>14.80388652533145</v>
       </c>
       <c r="AE5" t="n">
-        <v>13.01066302075827</v>
+        <v>13.52815369651853</v>
       </c>
       <c r="AF5" t="n">
-        <v>13.60938050526429</v>
+        <v>14.09385429581628</v>
       </c>
       <c r="AG5" t="n">
-        <v>13.55204714920824</v>
+        <v>13.99561052747057</v>
       </c>
       <c r="AH5" t="n">
-        <v>14.05255256714645</v>
+        <v>14.29488143933609</v>
       </c>
       <c r="AI5" t="n">
-        <v>12.91529568976691</v>
+        <v>13.44268444380788</v>
       </c>
       <c r="AJ5" t="n">
-        <v>12.97428961100479</v>
+        <v>13.46425215493992</v>
       </c>
       <c r="AK5" t="n">
-        <v>13.05366283618727</v>
+        <v>13.54576753394172</v>
       </c>
       <c r="AL5" t="n">
-        <v>13.201243943768</v>
+        <v>13.75471559785692</v>
       </c>
       <c r="AM5" t="n">
-        <v>12.68295605248084</v>
+        <v>13.24179223453048</v>
       </c>
       <c r="AN5" t="n">
-        <v>13.18110940987493</v>
+        <v>13.7570482481713</v>
       </c>
       <c r="AO5" t="n">
-        <v>13.38841339916432</v>
+        <v>13.88403184576414</v>
       </c>
       <c r="AP5" t="n">
-        <v>12.92846294305989</v>
+        <v>13.41592768834035</v>
       </c>
       <c r="AQ5" t="n">
-        <v>12.96042166473481</v>
+        <v>13.49663524774501</v>
       </c>
       <c r="AR5" t="n">
-        <v>13.08244194568382</v>
+        <v>13.53995666653879</v>
       </c>
       <c r="AS5" t="n">
-        <v>15.48131272652438</v>
+        <v>15.55358183405551</v>
       </c>
       <c r="AT5" t="n">
-        <v>13.98635641871022</v>
+        <v>14.30779599456618</v>
       </c>
       <c r="AU5" t="n">
-        <v>12.85649346750653</v>
+        <v>13.38753285424104</v>
       </c>
       <c r="AV5" t="n">
-        <v>12.9179961389748</v>
+        <v>13.45158040162726</v>
       </c>
       <c r="AW5" t="n">
-        <v>13.60267597815453</v>
+        <v>13.93277594557236</v>
       </c>
       <c r="AX5" t="n">
-        <v>12.83014053564217</v>
+        <v>13.44511075549492</v>
       </c>
       <c r="AY5" t="n">
-        <v>13.25565485219543</v>
+        <v>13.77603704090597</v>
       </c>
       <c r="AZ5" t="n">
-        <v>13.1325100356216</v>
+        <v>13.54179215361327</v>
       </c>
       <c r="BA5" t="n">
-        <v>12.79563640521148</v>
+        <v>13.32859015798411</v>
       </c>
       <c r="BB5" t="n">
-        <v>12.76306458906265</v>
+        <v>13.33112200024611</v>
       </c>
       <c r="BC5" t="n">
-        <v>13.30132510375159</v>
+        <v>13.7793154924488</v>
       </c>
       <c r="BD5" t="n">
-        <v>13.38630252065056</v>
+        <v>13.82457899053938</v>
       </c>
       <c r="BE5" t="n">
-        <v>13.25352127062284</v>
+        <v>13.80364592382406</v>
       </c>
       <c r="BF5" t="n">
-        <v>13.25618221627057</v>
+        <v>13.68828045066345</v>
       </c>
       <c r="BG5" t="n">
-        <v>12.98206614475731</v>
+        <v>13.32249044931731</v>
       </c>
       <c r="BH5" t="n">
-        <v>13.06555704177839</v>
+        <v>13.52575429222629</v>
       </c>
       <c r="BI5" t="n">
-        <v>13.16248107709187</v>
+        <v>13.66902952522735</v>
       </c>
       <c r="BJ5" t="n">
-        <v>13.09592259541551</v>
+        <v>13.6585356283445</v>
       </c>
       <c r="BK5" t="n">
-        <v>13.02238845764625</v>
+        <v>13.60374306086111</v>
       </c>
       <c r="BL5" t="n">
-        <v>13.41865499437346</v>
+        <v>13.91850972413718</v>
       </c>
       <c r="BM5" t="n">
-        <v>13.34496694548082</v>
+        <v>13.89812384731689</v>
       </c>
       <c r="BN5" t="n">
-        <v>13.11675546686555</v>
+        <v>13.58127804989314</v>
       </c>
       <c r="BO5" t="n">
-        <v>13.04792026535202</v>
+        <v>13.69133066208371</v>
       </c>
       <c r="BP5" t="n">
-        <v>13.66127332238749</v>
+        <v>14.23129173558764</v>
       </c>
       <c r="BQ5" t="n">
-        <v>12.92761171819844</v>
+        <v>13.35053348820745</v>
       </c>
       <c r="BR5" t="n">
-        <v>12.93791215148589</v>
+        <v>13.41770696159747</v>
       </c>
       <c r="BS5" t="n">
-        <v>13.13015132480932</v>
+        <v>13.59761688113856</v>
       </c>
       <c r="BT5" t="n">
-        <v>13.07683266770756</v>
+        <v>13.62373526667</v>
       </c>
       <c r="BU5" t="n">
-        <v>14.31876473303616</v>
+        <v>14.72884785523591</v>
       </c>
       <c r="BV5" t="n">
-        <v>13.94445339860146</v>
+        <v>14.23638410186375</v>
       </c>
       <c r="BW5" t="n">
-        <v>12.84638387776795</v>
+        <v>13.33814602360922</v>
       </c>
       <c r="BX5" t="n">
-        <v>13.31690743708587</v>
+        <v>13.74646184998742</v>
       </c>
       <c r="BY5" t="n">
-        <v>12.96384314230772</v>
+        <v>13.44436483884925</v>
       </c>
       <c r="BZ5" t="n">
-        <v>13.10663702810304</v>
+        <v>13.54071442126967</v>
       </c>
       <c r="CA5" t="n">
-        <v>13.28838486316792</v>
+        <v>13.69459006707135</v>
       </c>
       <c r="CB5" t="n">
-        <v>13.34584349089248</v>
+        <v>13.84752735539905</v>
       </c>
       <c r="CC5" t="n">
-        <v>12.72608418232308</v>
+        <v>13.19873850161938</v>
       </c>
       <c r="CD5" t="n">
-        <v>13.21370540420856</v>
+        <v>13.57046813802075</v>
       </c>
       <c r="CE5" t="n">
-        <v>13.24664961674842</v>
+        <v>13.76175954285624</v>
       </c>
       <c r="CF5" t="n">
-        <v>13.76205549959451</v>
+        <v>14.17853375717155</v>
       </c>
       <c r="CG5" t="n">
-        <v>13.05304900463782</v>
+        <v>13.62386865655924</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>13.39361525079328</v>
+        <v>13.16897384983088</v>
       </c>
       <c r="B6" t="n">
-        <v>12.08087428812427</v>
+        <v>11.48431410239292</v>
       </c>
       <c r="C6" t="n">
-        <v>11.82010288083968</v>
+        <v>11.7256796354345</v>
       </c>
       <c r="D6" t="n">
-        <v>11.15483153464485</v>
+        <v>11.29755843624699</v>
       </c>
       <c r="E6" t="n">
-        <v>12.1140641986401</v>
+        <v>12.56295671115582</v>
       </c>
       <c r="F6" t="n">
-        <v>12.03559733597134</v>
+        <v>12.46055344873248</v>
       </c>
       <c r="G6" t="n">
-        <v>12.55691310394519</v>
+        <v>12.94493851131149</v>
       </c>
       <c r="H6" t="n">
-        <v>12.55901061675454</v>
+        <v>12.95297134755863</v>
       </c>
       <c r="I6" t="n">
-        <v>13.15998623844978</v>
+        <v>13.59091308344581</v>
       </c>
       <c r="J6" t="n">
-        <v>12.22988604867248</v>
+        <v>12.69357777742587</v>
       </c>
       <c r="K6" t="n">
-        <v>12.25288078998597</v>
+        <v>12.68871294569226</v>
       </c>
       <c r="L6" t="n">
-        <v>12.03517568817034</v>
+        <v>12.73964401888264</v>
       </c>
       <c r="M6" t="n">
-        <v>12.02046655113118</v>
+        <v>12.71603629258379</v>
       </c>
       <c r="N6" t="n">
-        <v>13.08681531043615</v>
+        <v>13.50501453847389</v>
       </c>
       <c r="O6" t="n">
-        <v>11.2464431169115</v>
+        <v>12.08641709855979</v>
       </c>
       <c r="P6" t="n">
-        <v>11.93751027103158</v>
+        <v>12.53020616043926</v>
       </c>
       <c r="Q6" t="n">
-        <v>15.13476718104493</v>
+        <v>14.76758485210411</v>
       </c>
       <c r="R6" t="n">
-        <v>12.13133280955217</v>
+        <v>12.80009796306748</v>
       </c>
       <c r="S6" t="n">
-        <v>12.69261545821726</v>
+        <v>13.31812139732456</v>
       </c>
       <c r="T6" t="n">
-        <v>12.78523862744473</v>
+        <v>13.37813110015592</v>
       </c>
       <c r="U6" t="n">
-        <v>11.36424204629208</v>
+        <v>12.1792806132597</v>
       </c>
       <c r="V6" t="n">
-        <v>11.4596250704594</v>
+        <v>12.26649865258572</v>
       </c>
       <c r="W6" t="n">
-        <v>11.38541632546058</v>
+        <v>12.17975913686391</v>
       </c>
       <c r="X6" t="n">
-        <v>12.38327015778068</v>
+        <v>12.98996029006121</v>
       </c>
       <c r="Y6" t="n">
-        <v>13.15110548985071</v>
+        <v>13.81863840661084</v>
       </c>
       <c r="Z6" t="n">
-        <v>12.25760098259721</v>
+        <v>12.93156335697769</v>
       </c>
       <c r="AA6" t="n">
-        <v>12.23228546918993</v>
+        <v>12.83380594535818</v>
       </c>
       <c r="AB6" t="n">
-        <v>12.21396678828783</v>
+        <v>12.86165866088828</v>
       </c>
       <c r="AC6" t="n">
-        <v>10.94152617424041</v>
+        <v>11.81086971426406</v>
       </c>
       <c r="AD6" t="n">
-        <v>13.0081615501085</v>
+        <v>13.73772339247585</v>
       </c>
       <c r="AE6" t="n">
-        <v>12.17721773726124</v>
+        <v>12.78847022544923</v>
       </c>
       <c r="AF6" t="n">
-        <v>12.8286707378929</v>
+        <v>13.38931595210811</v>
       </c>
       <c r="AG6" t="n">
-        <v>12.79374734240641</v>
+        <v>13.29137103681074</v>
       </c>
       <c r="AH6" t="n">
-        <v>13.44516143406113</v>
+        <v>13.67931039823211</v>
       </c>
       <c r="AI6" t="n">
-        <v>11.90139757335961</v>
+        <v>12.55030619305704</v>
       </c>
       <c r="AJ6" t="n">
-        <v>12.01629290918239</v>
+        <v>12.61574113384136</v>
       </c>
       <c r="AK6" t="n">
-        <v>12.23957799614066</v>
+        <v>12.80828719516641</v>
       </c>
       <c r="AL6" t="n">
-        <v>12.31200395971845</v>
+        <v>12.96475799096101</v>
       </c>
       <c r="AM6" t="n">
-        <v>11.66504896955378</v>
+        <v>12.33885787764673</v>
       </c>
       <c r="AN6" t="n">
-        <v>12.02545363737578</v>
+        <v>12.71858720006638</v>
       </c>
       <c r="AO6" t="n">
-        <v>12.66330921564067</v>
+        <v>13.21896735894927</v>
       </c>
       <c r="AP6" t="n">
-        <v>11.93636076090846</v>
+        <v>12.50190331614688</v>
       </c>
       <c r="AQ6" t="n">
-        <v>12.01081444493173</v>
+        <v>12.65796909865951</v>
       </c>
       <c r="AR6" t="n">
-        <v>12.19718767323769</v>
+        <v>12.69242724569544</v>
       </c>
       <c r="AS6" t="n">
-        <v>15.66385194167859</v>
+        <v>15.6020270136389</v>
       </c>
       <c r="AT6" t="n">
-        <v>13.49747132328312</v>
+        <v>13.78505936690012</v>
       </c>
       <c r="AU6" t="n">
-        <v>11.89218150956475</v>
+        <v>12.51265225134554</v>
       </c>
       <c r="AV6" t="n">
-        <v>11.89858745532628</v>
+        <v>12.54467421818975</v>
       </c>
       <c r="AW6" t="n">
-        <v>12.96645598738736</v>
+        <v>13.29823151078175</v>
       </c>
       <c r="AX6" t="n">
-        <v>11.68211875825202</v>
+        <v>12.42697205917919</v>
       </c>
       <c r="AY6" t="n">
-        <v>12.38968971292261</v>
+        <v>12.99631484726404</v>
       </c>
       <c r="AZ6" t="n">
-        <v>12.32765912893465</v>
+        <v>12.75498038311126</v>
       </c>
       <c r="BA6" t="n">
-        <v>11.80049294862772</v>
+        <v>12.4296179461456</v>
       </c>
       <c r="BB6" t="n">
-        <v>11.77520668269205</v>
+        <v>12.45046797012258</v>
       </c>
       <c r="BC6" t="n">
-        <v>12.50042556781475</v>
+        <v>13.04627003716337</v>
       </c>
       <c r="BD6" t="n">
-        <v>12.71861186138172</v>
+        <v>13.1664503476807</v>
       </c>
       <c r="BE6" t="n">
-        <v>12.39491653750808</v>
+        <v>13.04563796321319</v>
       </c>
       <c r="BF6" t="n">
-        <v>12.53261206348661</v>
+        <v>12.96375507756549</v>
       </c>
       <c r="BG6" t="n">
-        <v>12.17281887757758</v>
+        <v>12.50147011307904</v>
       </c>
       <c r="BH6" t="n">
-        <v>12.18782279340746</v>
+        <v>12.70827060140956</v>
       </c>
       <c r="BI6" t="n">
-        <v>12.2788450723154</v>
+        <v>12.87726747102027</v>
       </c>
       <c r="BJ6" t="n">
-        <v>12.1695241299313</v>
+        <v>12.83075476134288</v>
       </c>
       <c r="BK6" t="n">
-        <v>11.88524245600074</v>
+        <v>12.60702407982996</v>
       </c>
       <c r="BL6" t="n">
-        <v>12.7122948919824</v>
+        <v>13.24196990161589</v>
       </c>
       <c r="BM6" t="n">
-        <v>12.33561366632934</v>
+        <v>13.00391983604216</v>
       </c>
       <c r="BN6" t="n">
-        <v>12.29646610269634</v>
+        <v>12.80384437973893</v>
       </c>
       <c r="BO6" t="n">
-        <v>11.91511512340995</v>
+        <v>12.68688629416595</v>
       </c>
       <c r="BP6" t="n">
-        <v>12.48984885698981</v>
+        <v>13.16508814593129</v>
       </c>
       <c r="BQ6" t="n">
-        <v>11.94678800641464</v>
+        <v>12.45241886369893</v>
       </c>
       <c r="BR6" t="n">
-        <v>12.00718550492499</v>
+        <v>12.56452016859112</v>
       </c>
       <c r="BS6" t="n">
-        <v>12.32479046955389</v>
+        <v>12.81957650427603</v>
       </c>
       <c r="BT6" t="n">
-        <v>12.04222259659974</v>
+        <v>12.6967947259671</v>
       </c>
       <c r="BU6" t="n">
-        <v>13.10538996541984</v>
+        <v>13.64710110557928</v>
       </c>
       <c r="BV6" t="n">
-        <v>13.51344519117909</v>
+        <v>13.74972342904826</v>
       </c>
       <c r="BW6" t="n">
-        <v>11.907748609319</v>
+        <v>12.47889765605736</v>
       </c>
       <c r="BX6" t="n">
-        <v>12.581709240287</v>
+        <v>13.03198340341042</v>
       </c>
       <c r="BY6" t="n">
-        <v>12.04228435175428</v>
+        <v>12.60149283870921</v>
       </c>
       <c r="BZ6" t="n">
-        <v>12.28859689081587</v>
+        <v>12.75076461849486</v>
       </c>
       <c r="CA6" t="n">
-        <v>12.58873492604809</v>
+        <v>13.00495118828796</v>
       </c>
       <c r="CB6" t="n">
-        <v>12.58032424340136</v>
+        <v>13.13831433120889</v>
       </c>
       <c r="CC6" t="n">
-        <v>11.75081046603172</v>
+        <v>12.29342098493361</v>
       </c>
       <c r="CD6" t="n">
-        <v>12.39315654983781</v>
+        <v>12.77623911314117</v>
       </c>
       <c r="CE6" t="n">
-        <v>12.25396637565338</v>
+        <v>12.86971213390362</v>
       </c>
       <c r="CF6" t="n">
-        <v>13.14161179509349</v>
+        <v>13.5833391782211</v>
       </c>
       <c r="CG6" t="n">
-        <v>12.10707661873275</v>
+        <v>12.79002772907886</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>12.51308813025587</v>
+        <v>12.32183241473159</v>
       </c>
       <c r="B7" t="n">
-        <v>11.51086763391551</v>
+        <v>10.8485697490405</v>
       </c>
       <c r="C7" t="n">
-        <v>11.30406566143964</v>
+        <v>11.12010049231351</v>
       </c>
       <c r="D7" t="n">
-        <v>10.24012589312923</v>
+        <v>10.2035664190141</v>
       </c>
       <c r="E7" t="n">
-        <v>11.27906568022004</v>
+        <v>11.51867748062635</v>
       </c>
       <c r="F7" t="n">
-        <v>11.07475956863385</v>
+        <v>11.24530432537503</v>
       </c>
       <c r="G7" t="n">
-        <v>11.58894067877358</v>
+        <v>11.72359183247844</v>
       </c>
       <c r="H7" t="n">
-        <v>11.45133485967044</v>
+        <v>11.56499164664643</v>
       </c>
       <c r="I7" t="n">
-        <v>12.0544400446375</v>
+        <v>12.1630651012197</v>
       </c>
       <c r="J7" t="n">
-        <v>10.9838495688142</v>
+        <v>11.11813915269153</v>
       </c>
       <c r="K7" t="n">
-        <v>11.12598709261415</v>
+        <v>11.12212882083278</v>
       </c>
       <c r="L7" t="n">
-        <v>10.62465723310033</v>
+        <v>11.00886772976914</v>
       </c>
       <c r="M7" t="n">
-        <v>10.55679529120782</v>
+        <v>10.95298319004891</v>
       </c>
       <c r="N7" t="n">
-        <v>11.8444802900652</v>
+        <v>11.96835518167088</v>
       </c>
       <c r="O7" t="n">
-        <v>9.795504515548343</v>
+        <v>10.37479917523665</v>
       </c>
       <c r="P7" t="n">
-        <v>10.40158491203357</v>
+        <v>10.786169457063</v>
       </c>
       <c r="Q7" t="n">
-        <v>14.1822656939482</v>
+        <v>13.36104880066598</v>
       </c>
       <c r="R7" t="n">
-        <v>10.58939572430659</v>
+        <v>10.96066232418125</v>
       </c>
       <c r="S7" t="n">
-        <v>11.38128877229558</v>
+        <v>11.71052188345149</v>
       </c>
       <c r="T7" t="n">
-        <v>11.26497506743432</v>
+        <v>11.61560046178797</v>
       </c>
       <c r="U7" t="n">
-        <v>9.780791733511602</v>
+        <v>10.29814152490406</v>
       </c>
       <c r="V7" t="n">
-        <v>9.99817591609661</v>
+        <v>10.48619552957057</v>
       </c>
       <c r="W7" t="n">
-        <v>9.969278458108157</v>
+        <v>10.43494675730689</v>
       </c>
       <c r="X7" t="n">
-        <v>10.86437700161821</v>
+        <v>11.16937476612735</v>
       </c>
       <c r="Y7" t="n">
-        <v>11.93717942540864</v>
+        <v>12.3391167165123</v>
       </c>
       <c r="Z7" t="n">
-        <v>10.77334261137592</v>
+        <v>11.12135885572056</v>
       </c>
       <c r="AA7" t="n">
-        <v>10.76071820043577</v>
+        <v>11.04948481514858</v>
       </c>
       <c r="AB7" t="n">
-        <v>10.73661110738479</v>
+        <v>11.07015929935548</v>
       </c>
       <c r="AC7" t="n">
-        <v>9.526186994424586</v>
+        <v>10.04015630639999</v>
       </c>
       <c r="AD7" t="n">
-        <v>11.82166556884509</v>
+        <v>12.23598894100726</v>
       </c>
       <c r="AE7" t="n">
-        <v>10.77539972615258</v>
+        <v>11.05917735687625</v>
       </c>
       <c r="AF7" t="n">
-        <v>11.46109179803725</v>
+        <v>11.69455438541467</v>
       </c>
       <c r="AG7" t="n">
-        <v>11.40281534234572</v>
+        <v>11.58682952719297</v>
       </c>
       <c r="AH7" t="n">
-        <v>12.35769015253392</v>
+        <v>12.25674253465991</v>
       </c>
       <c r="AI7" t="n">
-        <v>10.47846918092799</v>
+        <v>10.84605461610503</v>
       </c>
       <c r="AJ7" t="n">
-        <v>10.61353159102405</v>
+        <v>10.88880164784332</v>
       </c>
       <c r="AK7" t="n">
-        <v>10.87623293312959</v>
+        <v>11.11031860706857</v>
       </c>
       <c r="AL7" t="n">
-        <v>10.87498230212942</v>
+        <v>11.19159554745007</v>
       </c>
       <c r="AM7" t="n">
-        <v>10.23448653740156</v>
+        <v>10.56579806232442</v>
       </c>
       <c r="AN7" t="n">
-        <v>10.60651552696946</v>
+        <v>11.01586193707309</v>
       </c>
       <c r="AO7" t="n">
-        <v>11.33176301380729</v>
+        <v>11.54403848856361</v>
       </c>
       <c r="AP7" t="n">
-        <v>10.63175061001037</v>
+        <v>10.85615542188509</v>
       </c>
       <c r="AQ7" t="n">
-        <v>10.61145187684941</v>
+        <v>10.96140986975995</v>
       </c>
       <c r="AR7" t="n">
-        <v>10.94847270312431</v>
+        <v>11.06755292188797</v>
       </c>
       <c r="AS7" t="n">
-        <v>14.92127527920598</v>
+        <v>14.44970541611586</v>
       </c>
       <c r="AT7" t="n">
-        <v>12.32219553887452</v>
+        <v>12.22600328174626</v>
       </c>
       <c r="AU7" t="n">
-        <v>10.51354018992052</v>
+        <v>10.76971689183498</v>
       </c>
       <c r="AV7" t="n">
-        <v>10.46894794389578</v>
+        <v>10.78275385345468</v>
       </c>
       <c r="AW7" t="n">
-        <v>11.74916527352953</v>
+        <v>11.71517673439404</v>
       </c>
       <c r="AX7" t="n">
-        <v>10.22469384401437</v>
+        <v>10.66786300917866</v>
       </c>
       <c r="AY7" t="n">
-        <v>11.00494681905593</v>
+        <v>11.28810134208873</v>
       </c>
       <c r="AZ7" t="n">
-        <v>11.0627756663507</v>
+        <v>11.09413314071604</v>
       </c>
       <c r="BA7" t="n">
-        <v>10.42138226365253</v>
+        <v>10.70489966922118</v>
       </c>
       <c r="BB7" t="n">
-        <v>10.41615839277986</v>
+        <v>10.74881657871896</v>
       </c>
       <c r="BC7" t="n">
-        <v>11.16761889109543</v>
+        <v>11.37089913120487</v>
       </c>
       <c r="BD7" t="n">
-        <v>11.53852948354383</v>
+        <v>11.60081524670747</v>
       </c>
       <c r="BE7" t="n">
-        <v>11.00566933328366</v>
+        <v>11.33246360408412</v>
       </c>
       <c r="BF7" t="n">
-        <v>11.34432902995652</v>
+        <v>11.36114335303589</v>
       </c>
       <c r="BG7" t="n">
-        <v>10.97441447125735</v>
+        <v>10.91020987615275</v>
       </c>
       <c r="BH7" t="n">
-        <v>10.85037779596043</v>
+        <v>11.01419613509174</v>
       </c>
       <c r="BI7" t="n">
-        <v>10.89790643597924</v>
+        <v>11.16677606317551</v>
       </c>
       <c r="BJ7" t="n">
-        <v>10.76461837942421</v>
+        <v>11.0959919490945</v>
       </c>
       <c r="BK7" t="n">
-        <v>10.40643350805447</v>
+        <v>10.81252125297272</v>
       </c>
       <c r="BL7" t="n">
-        <v>11.45362569265229</v>
+        <v>11.59867400728414</v>
       </c>
       <c r="BM7" t="n">
-        <v>10.87121456578622</v>
+        <v>11.22729972913984</v>
       </c>
       <c r="BN7" t="n">
-        <v>11.02145842755334</v>
+        <v>11.15374077513969</v>
       </c>
       <c r="BO7" t="n">
-        <v>10.4855543012463</v>
+        <v>10.97544639844669</v>
       </c>
       <c r="BP7" t="n">
-        <v>11.14764705633151</v>
+        <v>11.56749883536518</v>
       </c>
       <c r="BQ7" t="n">
-        <v>10.56262337372869</v>
+        <v>10.74948040564087</v>
       </c>
       <c r="BR7" t="n">
-        <v>10.64703545691802</v>
+        <v>10.8541493232936</v>
       </c>
       <c r="BS7" t="n">
-        <v>11.05731551770272</v>
+        <v>11.16399450038642</v>
       </c>
       <c r="BT7" t="n">
-        <v>10.58472418493131</v>
+        <v>10.92242433207201</v>
       </c>
       <c r="BU7" t="n">
-        <v>11.81977203418213</v>
+        <v>12.06718755162789</v>
       </c>
       <c r="BV7" t="n">
-        <v>12.42800014463231</v>
+        <v>12.27411082679723</v>
       </c>
       <c r="BW7" t="n">
-        <v>10.57891208783301</v>
+        <v>10.80088558020708</v>
       </c>
       <c r="BX7" t="n">
-        <v>11.35080678904675</v>
+        <v>11.4169101676061</v>
       </c>
       <c r="BY7" t="n">
-        <v>10.6823815712952</v>
+        <v>10.89939145386368</v>
       </c>
       <c r="BZ7" t="n">
-        <v>11.02071774400314</v>
+        <v>11.09164320308315</v>
       </c>
       <c r="CA7" t="n">
-        <v>11.41484378901537</v>
+        <v>11.46015955576683</v>
       </c>
       <c r="CB7" t="n">
-        <v>11.27966854154201</v>
+        <v>11.47806878427001</v>
       </c>
       <c r="CC7" t="n">
-        <v>10.42240792635148</v>
+        <v>10.5868997832305</v>
       </c>
       <c r="CD7" t="n">
-        <v>11.07489686309069</v>
+        <v>11.10482755685982</v>
       </c>
       <c r="CE7" t="n">
-        <v>10.82183086164472</v>
+        <v>11.12762919934714</v>
       </c>
       <c r="CF7" t="n">
-        <v>11.87082663758833</v>
+        <v>11.94066836360836</v>
       </c>
       <c r="CG7" t="n">
-        <v>10.65736035669552</v>
+        <v>10.98681444808681</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15.13000552727541</v>
+        <v>14.94320807916739</v>
       </c>
       <c r="B8" t="n">
-        <v>13.05653156113744</v>
+        <v>12.43228552316051</v>
       </c>
       <c r="C8" t="n">
-        <v>13.59630409127087</v>
+        <v>13.48932125358357</v>
       </c>
       <c r="D8" t="n">
-        <v>12.323875495742</v>
+        <v>12.48203767708312</v>
       </c>
       <c r="E8" t="n">
-        <v>13.64690922611024</v>
+        <v>14.17724386535593</v>
       </c>
       <c r="F8" t="n">
-        <v>13.27369067806147</v>
+        <v>13.69725304114789</v>
       </c>
       <c r="G8" t="n">
-        <v>13.95832343330569</v>
+        <v>14.30679099598136</v>
       </c>
       <c r="H8" t="n">
-        <v>13.27039975729387</v>
+        <v>13.67124196977701</v>
       </c>
       <c r="I8" t="n">
-        <v>14.39269403847823</v>
+        <v>14.73388712234058</v>
       </c>
       <c r="J8" t="n">
-        <v>12.9774640871267</v>
+        <v>13.39091541176987</v>
       </c>
       <c r="K8" t="n">
-        <v>12.8560158574747</v>
+        <v>13.28277033954006</v>
       </c>
       <c r="L8" t="n">
-        <v>12.94153009462596</v>
+        <v>13.63341419449901</v>
       </c>
       <c r="M8" t="n">
-        <v>13.00933374567067</v>
+        <v>13.66316973103541</v>
       </c>
       <c r="N8" t="n">
-        <v>13.4520652361515</v>
+        <v>13.86233077626042</v>
       </c>
       <c r="O8" t="n">
-        <v>12.08493535581568</v>
+        <v>12.83173115317775</v>
       </c>
       <c r="P8" t="n">
-        <v>12.65338526179465</v>
+        <v>13.21042098515022</v>
       </c>
       <c r="Q8" t="n">
-        <v>15.2668986506985</v>
+        <v>14.94991126168263</v>
       </c>
       <c r="R8" t="n">
-        <v>12.83738042513829</v>
+        <v>13.42826963898626</v>
       </c>
       <c r="S8" t="n">
-        <v>13.83912976194062</v>
+        <v>14.40041418042211</v>
       </c>
       <c r="T8" t="n">
-        <v>13.52941736989466</v>
+        <v>14.08197635859346</v>
       </c>
       <c r="U8" t="n">
-        <v>12.0600012486701</v>
+        <v>12.8037920198432</v>
       </c>
       <c r="V8" t="n">
-        <v>12.28679813431229</v>
+        <v>12.99981966417079</v>
       </c>
       <c r="W8" t="n">
-        <v>12.22455825001313</v>
+        <v>12.91788708118256</v>
       </c>
       <c r="X8" t="n">
-        <v>13.12736974208307</v>
+        <v>13.64271997006806</v>
       </c>
       <c r="Y8" t="n">
-        <v>14.22555464159614</v>
+        <v>14.79550458710653</v>
       </c>
       <c r="Z8" t="n">
-        <v>12.98093855646628</v>
+        <v>13.55719048239906</v>
       </c>
       <c r="AA8" t="n">
-        <v>12.88022838604612</v>
+        <v>13.40208743131151</v>
       </c>
       <c r="AB8" t="n">
-        <v>13.02032438683128</v>
+        <v>13.56075170515833</v>
       </c>
       <c r="AC8" t="n">
-        <v>11.81760011497567</v>
+        <v>12.58954094469186</v>
       </c>
       <c r="AD8" t="n">
-        <v>14.2256009185273</v>
+        <v>14.83936865409372</v>
       </c>
       <c r="AE8" t="n">
-        <v>12.84032303251159</v>
+        <v>13.33828138819066</v>
       </c>
       <c r="AF8" t="n">
-        <v>13.58586500759564</v>
+        <v>14.03195511947352</v>
       </c>
       <c r="AG8" t="n">
-        <v>13.39337111238126</v>
+        <v>13.82059648361759</v>
       </c>
       <c r="AH8" t="n">
-        <v>13.73640014995851</v>
+        <v>13.93596990432848</v>
       </c>
       <c r="AI8" t="n">
-        <v>12.6679535534524</v>
+        <v>13.22616572105358</v>
       </c>
       <c r="AJ8" t="n">
-        <v>12.78148998288232</v>
+        <v>13.27008112503471</v>
       </c>
       <c r="AK8" t="n">
-        <v>12.87330485374735</v>
+        <v>13.34330122599407</v>
       </c>
       <c r="AL8" t="n">
-        <v>13.0206538258983</v>
+        <v>13.55325670798975</v>
       </c>
       <c r="AM8" t="n">
-        <v>12.43209330634218</v>
+        <v>13.00986683133087</v>
       </c>
       <c r="AN8" t="n">
-        <v>12.99307059778788</v>
+        <v>13.60300925678283</v>
       </c>
       <c r="AO8" t="n">
-        <v>13.20372978863228</v>
+        <v>13.67408443780004</v>
       </c>
       <c r="AP8" t="n">
-        <v>12.58948218019602</v>
+        <v>13.08175352591837</v>
       </c>
       <c r="AQ8" t="n">
-        <v>12.66455936234533</v>
+        <v>13.21238201637654</v>
       </c>
       <c r="AR8" t="n">
-        <v>12.85220455915427</v>
+        <v>13.28329394209133</v>
       </c>
       <c r="AS8" t="n">
-        <v>15.73203396934786</v>
+        <v>15.66721599408371</v>
       </c>
       <c r="AT8" t="n">
-        <v>13.88647974578109</v>
+        <v>14.13775465475506</v>
       </c>
       <c r="AU8" t="n">
-        <v>12.57439208231537</v>
+        <v>13.09768365971864</v>
       </c>
       <c r="AV8" t="n">
-        <v>12.68339587221483</v>
+        <v>13.21822689977945</v>
       </c>
       <c r="AW8" t="n">
-        <v>13.45614607952234</v>
+        <v>13.73624412772153</v>
       </c>
       <c r="AX8" t="n">
-        <v>12.58937857775599</v>
+        <v>13.24099980832631</v>
       </c>
       <c r="AY8" t="n">
-        <v>13.07526475011409</v>
+        <v>13.57988975288399</v>
       </c>
       <c r="AZ8" t="n">
-        <v>12.89976162943633</v>
+        <v>13.26321575019857</v>
       </c>
       <c r="BA8" t="n">
-        <v>12.53174398577761</v>
+        <v>13.06522413821171</v>
       </c>
       <c r="BB8" t="n">
-        <v>12.48742487563329</v>
+        <v>13.05799701436492</v>
       </c>
       <c r="BC8" t="n">
-        <v>13.1043346510385</v>
+        <v>13.56252499080581</v>
       </c>
       <c r="BD8" t="n">
-        <v>13.20766897570619</v>
+        <v>13.58687575222428</v>
       </c>
       <c r="BE8" t="n">
-        <v>13.05918837754716</v>
+        <v>13.59571561641412</v>
       </c>
       <c r="BF8" t="n">
-        <v>13.04122137637098</v>
+        <v>13.3977528580814</v>
       </c>
       <c r="BG8" t="n">
-        <v>12.75380360307882</v>
+        <v>13.0337946226837</v>
       </c>
       <c r="BH8" t="n">
-        <v>12.83132821655871</v>
+        <v>13.2728534135901</v>
       </c>
       <c r="BI8" t="n">
-        <v>12.96008487974537</v>
+        <v>13.45167578125228</v>
       </c>
       <c r="BJ8" t="n">
-        <v>12.88449905523877</v>
+        <v>13.44023131411995</v>
       </c>
       <c r="BK8" t="n">
-        <v>12.79621535791142</v>
+        <v>13.40236197117214</v>
       </c>
       <c r="BL8" t="n">
-        <v>13.20397367307479</v>
+        <v>13.64667800275649</v>
       </c>
       <c r="BM8" t="n">
-        <v>13.17595315497633</v>
+        <v>13.74188138503915</v>
       </c>
       <c r="BN8" t="n">
-        <v>12.8784614653829</v>
+        <v>13.30689946290363</v>
       </c>
       <c r="BO8" t="n">
-        <v>12.84943407042758</v>
+        <v>13.53571647367742</v>
       </c>
       <c r="BP8" t="n">
-        <v>13.53186282077146</v>
+        <v>14.14511146979368</v>
       </c>
       <c r="BQ8" t="n">
-        <v>12.7199303855685</v>
+        <v>13.13033941760909</v>
       </c>
       <c r="BR8" t="n">
-        <v>12.68763165721899</v>
+        <v>13.15783221389566</v>
       </c>
       <c r="BS8" t="n">
-        <v>12.8820904915766</v>
+        <v>13.29838629767225</v>
       </c>
       <c r="BT8" t="n">
-        <v>12.87054042016942</v>
+        <v>13.43112514952225</v>
       </c>
       <c r="BU8" t="n">
-        <v>14.21968740599905</v>
+        <v>14.67428677490403</v>
       </c>
       <c r="BV8" t="n">
-        <v>13.87209553129333</v>
+        <v>14.07806289471178</v>
       </c>
       <c r="BW8" t="n">
-        <v>12.57649562865562</v>
+        <v>13.05487143573244</v>
       </c>
       <c r="BX8" t="n">
-        <v>13.12091099766921</v>
+        <v>13.50919502520581</v>
       </c>
       <c r="BY8" t="n">
-        <v>12.71560533082424</v>
+        <v>13.17873818045464</v>
       </c>
       <c r="BZ8" t="n">
-        <v>12.87645971929022</v>
+        <v>13.27637651906129</v>
       </c>
       <c r="CA8" t="n">
-        <v>13.1105563464271</v>
+        <v>13.46459037145132</v>
       </c>
       <c r="CB8" t="n">
-        <v>13.13274864407889</v>
+        <v>13.60015330398703</v>
       </c>
       <c r="CC8" t="n">
-        <v>12.43288630586998</v>
+        <v>12.89827483421606</v>
       </c>
       <c r="CD8" t="n">
-        <v>13.01985705079877</v>
+        <v>13.34709130509512</v>
       </c>
       <c r="CE8" t="n">
-        <v>13.08034986463835</v>
+        <v>13.60521958381909</v>
       </c>
       <c r="CF8" t="n">
-        <v>13.61006353002824</v>
+        <v>13.97958967981696</v>
       </c>
       <c r="CG8" t="n">
-        <v>12.80499716010064</v>
+        <v>13.37552977930304</v>
       </c>
     </row>
   </sheetData>

</xml_diff>